<commit_message>
changes made in excel file
</commit_message>
<xml_diff>
--- a/ARUBA/ITSA/Aruba_Jaguar_14_09_2015.xlsx
+++ b/ARUBA/ITSA/Aruba_Jaguar_14_09_2015.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavana\Documents\delivery-qa\ARUBA\ITSA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="630" windowWidth="19635" windowHeight="7440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="customcolumns" sheetId="7" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="90">
   <si>
     <t>ITSM_SYSTEM</t>
   </si>
@@ -543,6 +548,21 @@
                                 END; 
 -- END
 </t>
+  </si>
+  <si>
+    <t>sub_category_src_code</t>
+  </si>
+  <si>
+    <t>sub_category_src_key</t>
+  </si>
+  <si>
+    <t>dwh_d_incident</t>
+  </si>
+  <si>
+    <t>dwh_d_problem</t>
+  </si>
+  <si>
+    <t>short_description</t>
   </si>
 </sst>
 </file>
@@ -634,6 +654,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -681,7 +704,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -716,7 +739,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,20 +1049,36 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
@@ -1189,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>